<commit_message>
Update SOWC cleaned Edited High2.xlsx
</commit_message>
<xml_diff>
--- a/SOWC cleaned Edited High2.xlsx
+++ b/SOWC cleaned Edited High2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="245">
   <si>
     <t xml:space="preserve">Countries and Areas</t>
   </si>
@@ -707,9 +707,6 @@
     <t xml:space="preserve">Burkina Faso</t>
   </si>
   <si>
-    <t xml:space="preserve">x,p</t>
-  </si>
-  <si>
     <t xml:space="preserve">x</t>
   </si>
   <si>
@@ -725,13 +722,7 @@
     <t xml:space="preserve">Colombia</t>
   </si>
   <si>
-    <t xml:space="preserve">&gt;95</t>
-  </si>
-  <si>
     <t xml:space="preserve">Comoros</t>
-  </si>
-  <si>
-    <t xml:space="preserve">p</t>
   </si>
   <si>
     <t xml:space="preserve">Dominican Republic</t>
@@ -804,6 +795,9 @@
   </si>
   <si>
     <t xml:space="preserve">United Republic of Tanzania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x,p</t>
   </si>
   <si>
     <t xml:space="preserve">Viet Nam</t>
@@ -1236,10 +1230,10 @@
   </sheetPr>
   <dimension ref="A1:IA796"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BX1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="BZ1" activeCellId="0" sqref="BZ1"/>
-      <selection pane="bottomLeft" activeCell="CF23" activeCellId="0" sqref="CF23"/>
+      <selection pane="topLeft" activeCell="BX1" activeCellId="0" sqref="BX1"/>
+      <selection pane="bottomLeft" activeCell="CA14" activeCellId="0" sqref="CA14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1253,9 +1247,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="7.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="3.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="20" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="20" style="0" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="25" style="0" width="14.43"/>
   </cols>
   <sheetData>
@@ -2164,15 +2158,11 @@
       <c r="CE2" s="30" t="n">
         <v>76.4</v>
       </c>
-      <c r="CF2" s="27" t="s">
-        <v>212</v>
-      </c>
+      <c r="CF2" s="27"/>
       <c r="CG2" s="30" t="n">
         <v>57.3</v>
       </c>
-      <c r="CH2" s="27" t="s">
-        <v>212</v>
-      </c>
+      <c r="CH2" s="27"/>
       <c r="CI2" s="32" t="n">
         <v>56.99489</v>
       </c>
@@ -2456,19 +2446,19 @@
         <v>41.9</v>
       </c>
       <c r="GC2" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GD2" s="35" t="n">
         <v>18.6</v>
       </c>
       <c r="GE2" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GF2" s="36" t="n">
         <v>2.25268817204301</v>
       </c>
       <c r="GG2" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GH2" s="30" t="n">
         <v>38.4</v>
@@ -2498,19 +2488,19 @@
         <v>8.4</v>
       </c>
       <c r="GU2" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GV2" s="35" t="n">
         <v>36.9</v>
       </c>
       <c r="GW2" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GX2" s="36" t="n">
         <v>4.39285714285714</v>
       </c>
       <c r="GY2" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GZ2" s="30"/>
       <c r="HA2" s="33"/>
@@ -2562,7 +2552,7 @@
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="25" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C3" s="26" t="n">
         <v>23</v>
@@ -3157,7 +3147,7 @@
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
       <c r="B4" s="25" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C4" s="26" t="n">
         <v>68</v>
@@ -3794,7 +3784,7 @@
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C5" s="26" t="n">
         <v>19</v>
@@ -4361,19 +4351,19 @@
         <v>12.4</v>
       </c>
       <c r="GU5" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GV5" s="35" t="n">
         <v>49.8</v>
       </c>
       <c r="GW5" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GX5" s="36" t="n">
         <v>4.01612903225806</v>
       </c>
       <c r="GY5" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GZ5" s="30"/>
       <c r="HA5" s="33"/>
@@ -4451,7 +4441,7 @@
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
       <c r="B6" s="25" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C6" s="26" t="n">
         <v>106</v>
@@ -4675,8 +4665,8 @@
       <c r="BZ6" s="28" t="n">
         <v>100</v>
       </c>
-      <c r="CA6" s="27" t="s">
-        <v>218</v>
+      <c r="CA6" s="27" t="n">
+        <v>95</v>
       </c>
       <c r="CB6" s="27"/>
       <c r="CC6" s="27"/>
@@ -4686,9 +4676,7 @@
       <c r="CG6" s="30" t="n">
         <v>44.5</v>
       </c>
-      <c r="CH6" s="27" t="s">
-        <v>213</v>
-      </c>
+      <c r="CH6" s="27"/>
       <c r="CI6" s="32" t="n">
         <v>98.15518</v>
       </c>
@@ -4944,37 +4932,37 @@
         <v>19.4</v>
       </c>
       <c r="GC6" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GD6" s="30" t="n">
         <v>6.8</v>
       </c>
       <c r="GE6" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GF6" s="33" t="n">
         <v>2.85294117647059</v>
       </c>
       <c r="GG6" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GH6" s="30" t="n">
         <v>47</v>
       </c>
       <c r="GI6" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GJ6" s="30" t="n">
         <v>61</v>
       </c>
       <c r="GK6" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GL6" s="33" t="n">
         <v>1.29787234042553</v>
       </c>
       <c r="GM6" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GN6" s="30" t="n">
         <v>93.2</v>
@@ -4992,19 +4980,19 @@
         <v>14.8</v>
       </c>
       <c r="GU6" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GV6" s="30" t="n">
         <v>32</v>
       </c>
       <c r="GW6" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GX6" s="33" t="n">
         <v>2.16216216216216</v>
       </c>
       <c r="GY6" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GZ6" s="30"/>
       <c r="HA6" s="33"/>
@@ -5040,7 +5028,7 @@
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="25" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C7" s="26" t="n">
         <v>22</v>
@@ -5269,9 +5257,7 @@
       <c r="CE7" s="30" t="n">
         <v>50.7</v>
       </c>
-      <c r="CF7" s="27" t="s">
-        <v>220</v>
-      </c>
+      <c r="CF7" s="27"/>
       <c r="CG7" s="30"/>
       <c r="CH7" s="27"/>
       <c r="CI7" s="32" t="n">
@@ -5615,7 +5601,7 @@
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1"/>
       <c r="B8" s="25" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C8" s="26" t="n">
         <v>68</v>
@@ -6238,7 +6224,7 @@
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1"/>
       <c r="B9" s="25" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C9" s="26" t="n">
         <v>106</v>
@@ -6473,9 +6459,7 @@
       <c r="CG9" s="30" t="n">
         <v>30.9</v>
       </c>
-      <c r="CH9" s="27" t="s">
-        <v>220</v>
-      </c>
+      <c r="CH9" s="27"/>
       <c r="CI9" s="32" t="n">
         <v>97.46197</v>
       </c>
@@ -6871,7 +6855,7 @@
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1"/>
       <c r="B10" s="25" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C10" s="26" t="n">
         <v>51</v>
@@ -7352,109 +7336,109 @@
         <v>8.6</v>
       </c>
       <c r="FW10" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="FX10" s="30" t="n">
         <v>90.1</v>
       </c>
       <c r="FY10" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="FZ10" s="33" t="n">
         <v>10.4767441860465</v>
       </c>
       <c r="GA10" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GB10" s="30" t="n">
         <v>56.6</v>
       </c>
       <c r="GC10" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GD10" s="30" t="n">
         <v>26.5</v>
       </c>
       <c r="GE10" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GF10" s="33" t="n">
         <v>2.13584905660377</v>
       </c>
       <c r="GG10" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GH10" s="30" t="n">
         <v>41.6</v>
       </c>
       <c r="GI10" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GJ10" s="30" t="n">
         <v>50.3</v>
       </c>
       <c r="GK10" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GL10" s="33" t="n">
         <v>1.20913461538462</v>
       </c>
       <c r="GM10" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GN10" s="30" t="n">
         <v>71.46</v>
       </c>
       <c r="GO10" s="37" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="GP10" s="30" t="n">
         <v>96.12</v>
       </c>
       <c r="GQ10" s="37" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="GR10" s="33" t="n">
         <v>1.34508816120907</v>
       </c>
       <c r="GS10" s="37" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="GT10" s="30" t="n">
         <v>8.5</v>
       </c>
       <c r="GU10" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GV10" s="30" t="n">
         <v>36.8</v>
       </c>
       <c r="GW10" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GX10" s="33" t="n">
         <v>4.32941176470588</v>
       </c>
       <c r="GY10" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GZ10" s="30" t="n">
         <v>21.4</v>
       </c>
       <c r="HA10" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="HB10" s="30" t="n">
         <v>43.4</v>
       </c>
       <c r="HC10" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="HD10" s="33" t="n">
         <v>2.02803738317757</v>
       </c>
       <c r="HE10" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="HF10" s="30"/>
       <c r="HG10" s="30"/>
@@ -7482,7 +7466,7 @@
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1"/>
       <c r="B11" s="25" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C11" s="26" t="n">
         <v>35</v>
@@ -7725,9 +7709,7 @@
       <c r="CE11" s="30" t="n">
         <v>56.9</v>
       </c>
-      <c r="CF11" s="27" t="s">
-        <v>220</v>
-      </c>
+      <c r="CF11" s="27"/>
       <c r="CG11" s="30"/>
       <c r="CH11" s="27"/>
       <c r="CI11" s="32" t="n">
@@ -8031,19 +8013,19 @@
         <v>48.7</v>
       </c>
       <c r="GO11" s="37" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="GP11" s="30" t="n">
         <v>81.5</v>
       </c>
       <c r="GQ11" s="37" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="GR11" s="33" t="n">
         <v>1.6735112936345</v>
       </c>
       <c r="GS11" s="37" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="GT11" s="30"/>
       <c r="GU11" s="33"/>
@@ -8083,7 +8065,7 @@
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1"/>
       <c r="B12" s="25" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C12" s="26" t="n">
         <v>29</v>
@@ -8630,37 +8612,37 @@
         <v>59.7</v>
       </c>
       <c r="GO12" s="37" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="GP12" s="30" t="n">
         <v>79.9</v>
       </c>
       <c r="GQ12" s="37" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="GR12" s="33" t="n">
         <v>1.33835845896147</v>
       </c>
       <c r="GS12" s="37" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="GT12" s="35" t="n">
         <v>19.7</v>
       </c>
       <c r="GU12" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GV12" s="35" t="n">
         <v>47.7</v>
       </c>
       <c r="GW12" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GX12" s="36" t="n">
         <v>2.42131979695431</v>
       </c>
       <c r="GY12" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GZ12" s="30"/>
       <c r="HA12" s="33"/>
@@ -8738,7 +8720,7 @@
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1"/>
       <c r="B13" s="25" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C13" s="26" t="n">
         <v>66</v>
@@ -8979,9 +8961,7 @@
       <c r="CE13" s="30" t="n">
         <v>82.6</v>
       </c>
-      <c r="CF13" s="27" t="s">
-        <v>220</v>
-      </c>
+      <c r="CF13" s="27"/>
       <c r="CG13" s="30"/>
       <c r="CH13" s="27"/>
       <c r="CI13" s="32" t="n">
@@ -9375,7 +9355,7 @@
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1"/>
       <c r="B14" s="25" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C14" s="26" t="n">
         <v>92</v>
@@ -9918,13 +9898,13 @@
         <v>12.7</v>
       </c>
       <c r="GU14" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GV14" s="35" t="n">
         <v>43.7</v>
       </c>
       <c r="GW14" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GX14" s="36" t="n">
         <v>3.44094488188976</v>
@@ -10006,7 +9986,7 @@
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1"/>
       <c r="B15" s="25" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C15" s="26" t="n">
         <v>31</v>
@@ -10649,7 +10629,7 @@
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1"/>
       <c r="B16" s="25" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C16" s="26" t="n">
         <v>142</v>
@@ -11122,7 +11102,7 @@
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1"/>
       <c r="B17" s="25" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C17" s="26" t="n">
         <v>8</v>
@@ -11699,7 +11679,7 @@
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1"/>
       <c r="B18" s="25" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C18" s="26" t="n">
         <v>50</v>
@@ -11946,9 +11926,7 @@
       <c r="CG18" s="30" t="n">
         <v>5.5</v>
       </c>
-      <c r="CH18" s="27" t="s">
-        <v>220</v>
-      </c>
+      <c r="CH18" s="27"/>
       <c r="CI18" s="32" t="n">
         <v>78.41248</v>
       </c>
@@ -12216,19 +12194,19 @@
         <v>47.6</v>
       </c>
       <c r="GC18" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GD18" s="30" t="n">
         <v>43.6</v>
       </c>
       <c r="GE18" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GF18" s="33" t="n">
         <v>1.09174311926606</v>
       </c>
       <c r="GG18" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GH18" s="30" t="n">
         <v>10.5</v>
@@ -12246,19 +12224,19 @@
         <v>54.1</v>
       </c>
       <c r="GO18" s="37" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="GP18" s="30" t="n">
         <v>82.2</v>
       </c>
       <c r="GQ18" s="37" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="GR18" s="33" t="n">
         <v>1.51940850277264</v>
       </c>
       <c r="GS18" s="37" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="GT18" s="30" t="n">
         <v>9.9</v>
@@ -12310,7 +12288,7 @@
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1"/>
       <c r="B19" s="25" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C19" s="26" t="n">
         <v>133</v>
@@ -12735,55 +12713,55 @@
         <v>91.9</v>
       </c>
       <c r="FQ19" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="FR19" s="30" t="n">
         <v>93.8</v>
       </c>
       <c r="FS19" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="FT19" s="33" t="n">
         <v>1.02067464635473</v>
       </c>
       <c r="FU19" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="FV19" s="35" t="n">
         <v>88.6</v>
       </c>
       <c r="FW19" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="FX19" s="35" t="n">
         <v>99.2</v>
       </c>
       <c r="FY19" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="FZ19" s="36" t="n">
         <v>1.1196388261851</v>
       </c>
       <c r="GA19" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GB19" s="30" t="n">
         <v>21.9</v>
       </c>
       <c r="GC19" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GD19" s="30" t="n">
         <v>15.7</v>
       </c>
       <c r="GE19" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GF19" s="33" t="n">
         <v>1.39490445859873</v>
       </c>
       <c r="GG19" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GH19" s="30"/>
       <c r="GI19" s="33"/>
@@ -12807,19 +12785,19 @@
         <v>23.4</v>
       </c>
       <c r="GU19" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GV19" s="30" t="n">
         <v>47.8</v>
       </c>
       <c r="GW19" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GX19" s="33" t="n">
         <v>2.04273504273504</v>
       </c>
       <c r="GY19" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GZ19" s="30"/>
       <c r="HA19" s="33"/>
@@ -12853,7 +12831,7 @@
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1"/>
       <c r="B20" s="25" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C20" s="26" t="n">
         <v>51</v>
@@ -13079,8 +13057,8 @@
       <c r="BZ20" s="28" t="n">
         <v>500</v>
       </c>
-      <c r="CA20" s="27" t="s">
-        <v>218</v>
+      <c r="CA20" s="27" t="n">
+        <v>95</v>
       </c>
       <c r="CB20" s="27" t="n">
         <v>64</v>
@@ -13336,19 +13314,19 @@
         <v>83.1</v>
       </c>
       <c r="FQ20" s="33" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="FR20" s="30" t="n">
         <v>93.3</v>
       </c>
       <c r="FS20" s="33" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="FT20" s="33" t="n">
         <v>1.12274368231047</v>
       </c>
       <c r="FU20" s="33" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="FV20" s="30" t="n">
         <v>72.7</v>
@@ -13402,37 +13380,37 @@
         <v>61.3</v>
       </c>
       <c r="GU20" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GV20" s="35" t="n">
         <v>69.3</v>
       </c>
       <c r="GW20" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GX20" s="36" t="n">
         <v>1.1305057096248</v>
       </c>
       <c r="GY20" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GZ20" s="35" t="n">
         <v>54.8</v>
       </c>
       <c r="HA20" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="HB20" s="35" t="n">
         <v>67.4</v>
       </c>
       <c r="HC20" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="HD20" s="36" t="n">
         <v>1.22992700729927</v>
       </c>
       <c r="HE20" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="HF20" s="30"/>
       <c r="HG20" s="30"/>
@@ -13460,7 +13438,7 @@
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1"/>
       <c r="B21" s="25" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C21" s="26" t="n">
         <v>11</v>
@@ -14069,7 +14047,7 @@
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1"/>
       <c r="B22" s="25" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C22" s="26" t="n">
         <v>88</v>
@@ -14296,9 +14274,7 @@
       <c r="CG22" s="30" t="n">
         <v>50</v>
       </c>
-      <c r="CH22" s="27" t="s">
-        <v>213</v>
-      </c>
+      <c r="CH22" s="27"/>
       <c r="CI22" s="32" t="n">
         <v>98.04035</v>
       </c>
@@ -14510,19 +14486,19 @@
         <v>67.2</v>
       </c>
       <c r="FQ22" s="36" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="FR22" s="35" t="n">
         <v>88.7</v>
       </c>
       <c r="FS22" s="36" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="FT22" s="36" t="n">
         <v>1.31994047619048</v>
       </c>
       <c r="FU22" s="36" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="FV22" s="30"/>
       <c r="FW22" s="33"/>
@@ -14592,7 +14568,7 @@
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1"/>
       <c r="B23" s="25" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C23" s="26" t="n">
         <v>57</v>
@@ -15221,7 +15197,7 @@
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1"/>
       <c r="B24" s="25" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C24" s="26" t="n">
         <v>48</v>
@@ -15818,7 +15794,7 @@
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1"/>
       <c r="B25" s="25" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C25" s="26" t="n">
         <v>76</v>
@@ -16021,15 +15997,11 @@
       <c r="CE25" s="30" t="n">
         <v>54.2</v>
       </c>
-      <c r="CF25" s="27" t="s">
-        <v>212</v>
-      </c>
+      <c r="CF25" s="27"/>
       <c r="CG25" s="30" t="n">
         <v>15.3</v>
       </c>
-      <c r="CH25" s="27" t="s">
-        <v>212</v>
-      </c>
+      <c r="CH25" s="27"/>
       <c r="CI25" s="32"/>
       <c r="CJ25" s="32"/>
       <c r="CK25" s="32" t="n">
@@ -16290,7 +16262,7 @@
       </c>
       <c r="GA25" s="33"/>
       <c r="GB25" s="30" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="GC25" s="33"/>
       <c r="GD25" s="30" t="n">
@@ -16321,37 +16293,37 @@
         <v>17.3</v>
       </c>
       <c r="GU25" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GV25" s="30" t="n">
         <v>36.5</v>
       </c>
       <c r="GW25" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GX25" s="33" t="n">
         <v>2.10982658959538</v>
       </c>
       <c r="GY25" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GZ25" s="30" t="n">
         <v>34.7</v>
       </c>
       <c r="HA25" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="HB25" s="30" t="n">
         <v>50.4</v>
       </c>
       <c r="HC25" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="HD25" s="33" t="n">
         <v>1.45244956772334</v>
       </c>
       <c r="HE25" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="HF25" s="30"/>
       <c r="HG25" s="30"/>
@@ -16379,7 +16351,7 @@
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1"/>
       <c r="B26" s="25" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C26" s="26" t="n">
         <v>92</v>
@@ -16878,19 +16850,19 @@
         <v>4.8</v>
       </c>
       <c r="GU26" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GV26" s="30" t="n">
         <v>10.1</v>
       </c>
       <c r="GW26" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GX26" s="33" t="n">
         <v>2.10416666666667</v>
       </c>
       <c r="GY26" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GZ26" s="30"/>
       <c r="HA26" s="33"/>
@@ -16968,7 +16940,7 @@
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="1"/>
       <c r="B27" s="25" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C27" s="26" t="n">
         <v>88</v>
@@ -17201,9 +17173,7 @@
       <c r="CG27" s="30" t="n">
         <v>85.9</v>
       </c>
-      <c r="CH27" s="27" t="s">
-        <v>212</v>
-      </c>
+      <c r="CH27" s="27"/>
       <c r="CI27" s="32" t="n">
         <v>98.08572</v>
       </c>
@@ -17457,37 +17427,37 @@
         <v>82.8</v>
       </c>
       <c r="FW27" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="FX27" s="30" t="n">
         <v>94.1</v>
       </c>
       <c r="FY27" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="FZ27" s="33" t="n">
         <v>1.13647342995169</v>
       </c>
       <c r="GA27" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GB27" s="30" t="n">
         <v>13.4</v>
       </c>
       <c r="GC27" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GD27" s="30" t="n">
         <v>5.5</v>
       </c>
       <c r="GE27" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GF27" s="33" t="n">
         <v>2.43636363636364</v>
       </c>
       <c r="GG27" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GH27" s="30"/>
       <c r="GI27" s="33"/>
@@ -17511,19 +17481,19 @@
         <v>25.7</v>
       </c>
       <c r="GU27" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GV27" s="30" t="n">
         <v>51.5</v>
       </c>
       <c r="GW27" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GX27" s="33" t="n">
         <v>2.00389105058366</v>
       </c>
       <c r="GY27" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GZ27" s="30"/>
       <c r="HA27" s="33"/>
@@ -17601,7 +17571,7 @@
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="1"/>
       <c r="B28" s="25" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C28" s="26" t="n">
         <v>25</v>
@@ -18242,7 +18212,7 @@
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1"/>
       <c r="B29" s="25" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C29" s="26" t="n">
         <v>36</v>
@@ -18799,37 +18769,37 @@
         <v>38.9</v>
       </c>
       <c r="GU29" s="36" t="s">
-        <v>212</v>
+        <v>242</v>
       </c>
       <c r="GV29" s="35" t="n">
         <v>54.8</v>
       </c>
       <c r="GW29" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GX29" s="36" t="n">
         <v>1.40874035989717</v>
       </c>
       <c r="GY29" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="GZ29" s="35" t="n">
         <v>33.5</v>
       </c>
       <c r="HA29" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="HB29" s="35" t="n">
         <v>55.5</v>
       </c>
       <c r="HC29" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="HD29" s="36" t="n">
         <v>1.65671641791045</v>
       </c>
       <c r="HE29" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="HF29" s="30"/>
       <c r="HG29" s="30"/>
@@ -18857,7 +18827,7 @@
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1"/>
       <c r="B30" s="25" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C30" s="26" t="n">
         <v>82</v>
@@ -19472,7 +19442,7 @@
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1"/>
       <c r="B31" s="25" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C31" s="26" t="n">
         <v>37</v>

</xml_diff>